<commit_message>
need to clean up
</commit_message>
<xml_diff>
--- a/Results/all_manual_rankings.xlsx
+++ b/Results/all_manual_rankings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellataira/Library/Mobile Documents/com~apple~CloudDocs/Desktop/is4200/homework--5-ellataira/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BB0377-4C76-B34C-8600-A1A07135A0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7134B9A8-3F48-4946-B05B-4322B0010B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{FFF75AE6-1EAD-5F49-A371-81F01370B25A}"/>
   </bookViews>
@@ -2759,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3548C1-1A9A-AD4D-B9E0-F2ADD6109DB6}">
   <dimension ref="A1:D800"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A771" workbookViewId="0">
-      <selection activeCell="D799" sqref="D799"/>
+    <sheetView tabSelected="1" topLeftCell="A590" workbookViewId="0">
+      <selection activeCell="J601" sqref="J601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>